<commit_message>
Updated the remaining time for tasks
Updated the remaining time for tasks and created the burndown chart,
moving across all the data.
</commit_message>
<xml_diff>
--- a/Sprint Breakdowns.xlsx
+++ b/Sprint Breakdowns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20000" windowHeight="14820" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="100">
   <si>
     <t>Sprint Backlog Template</t>
   </si>
@@ -890,8 +890,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,7 +1293,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1345,6 +1363,15 @@
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1414,6 +1441,15 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2232,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T133"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="P69" sqref="A56:P69"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6484,9 +6520,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" s="37" customFormat="1" ht="19" customHeight="1"/>
-    <row r="127" s="21" customFormat="1"/>
-    <row r="128" s="21" customFormat="1"/>
+    <row r="116" spans="3:3">
+      <c r="C116">
+        <f>SUM(C15+C27+C41+C53+C67+C80+C95+C105) + 30</f>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" s="37" customFormat="1" ht="19" customHeight="1"/>
+    <row r="127" spans="3:3" s="21" customFormat="1"/>
+    <row r="128" spans="3:3" s="21" customFormat="1"/>
     <row r="129" s="21" customFormat="1"/>
     <row r="130" s="21" customFormat="1"/>
     <row r="131" s="21" customFormat="1"/>
@@ -8182,10 +8224,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8194,8 +8236,8 @@
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1"/>
-    <row r="2" spans="1:16" ht="20">
+    <row r="1" spans="1:12" ht="16" thickBot="1"/>
+    <row r="2" spans="1:12" ht="20">
       <c r="A2" s="27" t="s">
         <v>45</v>
       </c>
@@ -8208,14 +8250,10 @@
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="36">
+      <c r="K2" s="29"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="36">
       <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
@@ -8246,23 +8284,11 @@
       <c r="J3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="18">
+    </row>
+    <row r="4" spans="1:12" ht="18">
       <c r="A4" s="30"/>
       <c r="B4" s="40" t="s">
         <v>99</v>
@@ -8291,23 +8317,11 @@
       <c r="J4" s="20">
         <v>1</v>
       </c>
-      <c r="K4" s="20">
-        <v>1</v>
-      </c>
-      <c r="L4" s="20">
-        <v>1</v>
-      </c>
-      <c r="M4" s="20">
-        <v>1</v>
-      </c>
-      <c r="N4" s="20">
-        <v>1</v>
-      </c>
-      <c r="O4" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="18">
+      <c r="K4" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18">
       <c r="A5" s="30"/>
       <c r="B5" s="40" t="s">
         <v>92</v>
@@ -8330,7 +8344,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="110">
-        <f t="shared" ref="H5:O5" si="0">G5</f>
+        <f t="shared" ref="H5:K5" si="0">G5</f>
         <v>2</v>
       </c>
       <c r="I5" s="110">
@@ -8341,28 +8355,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K5" s="110">
+      <c r="K5" s="111">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L5" s="110">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M5" s="110">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N5" s="110">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O5" s="111">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="18">
+    </row>
+    <row r="6" spans="1:12" ht="18">
       <c r="A6" s="30"/>
       <c r="B6" s="40" t="s">
         <v>91</v>
@@ -8385,7 +8383,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="110">
-        <f t="shared" ref="H6:O6" si="2">G6</f>
+        <f t="shared" ref="H6:K6" si="2">G6</f>
         <v>4</v>
       </c>
       <c r="I6" s="110">
@@ -8396,28 +8394,12 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="K6" s="110">
+      <c r="K6" s="111">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="L6" s="110">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="M6" s="110">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="N6" s="110">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="O6" s="111">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="18">
+    </row>
+    <row r="7" spans="1:12" ht="18">
       <c r="A7" s="30"/>
       <c r="B7" s="39" t="s">
         <v>90</v>
@@ -8440,7 +8422,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="110">
-        <f t="shared" ref="H7:O7" si="3">G7</f>
+        <f t="shared" ref="H7:K7" si="3">G7</f>
         <v>3</v>
       </c>
       <c r="I7" s="110">
@@ -8451,28 +8433,12 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="K7" s="110">
+      <c r="K7" s="111">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L7" s="110">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M7" s="110">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="N7" s="110">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="O7" s="111">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="30">
+    </row>
+    <row r="8" spans="1:12" ht="30">
       <c r="A8" s="32"/>
       <c r="B8" s="39" t="s">
         <v>46</v>
@@ -8491,7 +8457,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="110">
-        <f t="shared" ref="G8:O20" si="4">F8</f>
+        <f t="shared" ref="G8:K20" si="4">F8</f>
         <v>2</v>
       </c>
       <c r="H8" s="110">
@@ -8506,29 +8472,13 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="K8" s="110">
+      <c r="K8" s="111">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="L8" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="M8" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="N8" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="O8" s="111">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="P8" s="21"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="32"/>
       <c r="B9" s="39" t="s">
         <v>83</v>
@@ -8562,29 +8512,13 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K9" s="110">
+      <c r="K9" s="111">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L9" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="M9" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N9" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="O9" s="111">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" ht="30">
+      <c r="L9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="32"/>
       <c r="B10" s="39" t="s">
         <v>39</v>
@@ -8618,29 +8552,13 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="K10" s="110">
+      <c r="K10" s="111">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="L10" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="M10" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="N10" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="O10" s="111">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" ht="30">
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" s="32"/>
       <c r="B11" s="39" t="s">
         <v>40</v>
@@ -8674,29 +8592,13 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="K11" s="110">
+      <c r="K11" s="111">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="L11" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="M11" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="N11" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="O11" s="111">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="32"/>
       <c r="B12" s="39" t="s">
         <v>85</v>
@@ -8730,29 +8632,13 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="K12" s="110">
+      <c r="K12" s="111">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="L12" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="M12" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="N12" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="O12" s="111">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="P12" s="21"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="32"/>
       <c r="B13" s="39" t="s">
         <v>47</v>
@@ -8786,29 +8672,13 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="K13" s="110">
+      <c r="K13" s="111">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="L13" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="M13" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="N13" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="O13" s="111">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="P13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" ht="30">
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" s="32"/>
       <c r="B14" s="39" t="s">
         <v>48</v>
@@ -8842,29 +8712,13 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="K14" s="110">
+      <c r="K14" s="111">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="L14" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="M14" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="N14" s="110">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="O14" s="111">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="33"/>
       <c r="B15" s="39" t="s">
         <v>86</v>
@@ -8898,29 +8752,13 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="K15" s="110">
+      <c r="K15" s="111">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="L15" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="M15" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="N15" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="O15" s="111">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="P15" s="21"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="33"/>
       <c r="B16" s="39" t="s">
         <v>87</v>
@@ -8954,29 +8792,13 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="K16" s="110">
+      <c r="K16" s="111">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="L16" s="110">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="M16" s="110">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="N16" s="110">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="O16" s="111">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="P16" s="21"/>
-    </row>
-    <row r="17" spans="1:16" ht="30">
+      <c r="L16" s="21"/>
+    </row>
+    <row r="17" spans="1:12" ht="30">
       <c r="A17" s="33"/>
       <c r="B17" s="39" t="s">
         <v>88</v>
@@ -9010,29 +8832,13 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K17" s="110">
+      <c r="K17" s="111">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L17" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="M17" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="N17" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="O17" s="111">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="P17" s="21"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="L17" s="21"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="33"/>
       <c r="B18" s="39" t="s">
         <v>89</v>
@@ -9066,29 +8872,13 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="K18" s="110">
+      <c r="K18" s="111">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="L18" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="M18" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="N18" s="110">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="O18" s="111">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="P18" s="21"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="33"/>
       <c r="B19" s="39" t="s">
         <v>96</v>
@@ -9122,29 +8912,13 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K19" s="110">
+      <c r="K19" s="111">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L19" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="M19" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="N19" s="110">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="O19" s="111">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="P19" s="21"/>
-    </row>
-    <row r="20" spans="1:16" ht="46" thickBot="1">
+      <c r="L19" s="21"/>
+    </row>
+    <row r="20" spans="1:12" ht="46" thickBot="1">
       <c r="A20" s="33"/>
       <c r="B20" s="45" t="s">
         <v>44</v>
@@ -9178,29 +8952,13 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K20" s="110">
+      <c r="K20" s="111">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L20" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="M20" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N20" s="110">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="111">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P20" s="21"/>
-    </row>
-    <row r="21" spans="1:16" ht="16" thickBot="1">
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="12" t="s">
         <v>15</v>
       </c>
@@ -9212,7 +8970,7 @@
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17">
-        <f t="shared" ref="F21:O21" si="5">SUM(F8:F20)</f>
+        <f t="shared" ref="F21:K21" si="5">SUM(F8:F20)</f>
         <v>47</v>
       </c>
       <c r="G21" s="17">
@@ -9231,29 +8989,13 @@
         <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="18">
         <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="L21" s="17">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-      <c r="M21" s="17">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-      <c r="N21" s="17">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-      <c r="O21" s="18">
-        <f t="shared" si="5"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="16" thickBot="1"/>
-    <row r="24" spans="1:16" ht="20">
+    </row>
+    <row r="23" spans="1:12" ht="16" thickBot="1"/>
+    <row r="24" spans="1:12" ht="20">
       <c r="A24" s="27" t="s">
         <v>49</v>
       </c>
@@ -9266,14 +9008,10 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" ht="36">
+      <c r="K24" s="29"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="36">
       <c r="A25" s="30" t="s">
         <v>1</v>
       </c>
@@ -9304,23 +9042,11 @@
       <c r="J25" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M25" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O25" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="30">
+    </row>
+    <row r="26" spans="1:12" ht="30">
       <c r="A26" s="32"/>
       <c r="B26" s="39" t="s">
         <v>50</v>
@@ -9339,44 +9065,27 @@
         <v>2</v>
       </c>
       <c r="G26" s="20">
-        <f>F26</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26" s="20">
-        <f t="shared" ref="H26:O41" si="6">G26</f>
-        <v>2</v>
+        <f t="shared" ref="H26:K41" si="6">G26</f>
+        <v>0</v>
       </c>
       <c r="I26" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="K26" s="20">
+        <v>0</v>
+      </c>
+      <c r="K26" s="44">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L26" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="M26" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="N26" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="O26" s="44">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="P26" s="21"/>
-    </row>
-    <row r="27" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" spans="1:12" ht="30">
       <c r="A27" s="32"/>
       <c r="B27" s="39" t="s">
         <v>61</v>
@@ -9391,48 +9100,31 @@
         <v>18</v>
       </c>
       <c r="F27" s="20">
-        <f>C27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G27" s="20">
         <f>F27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="K27" s="20">
+        <v>0</v>
+      </c>
+      <c r="K27" s="44">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L27" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="M27" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="N27" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="O27" s="44">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="P27" s="21"/>
-    </row>
-    <row r="28" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="32"/>
       <c r="B28" s="39" t="s">
         <v>83</v>
@@ -9455,40 +9147,22 @@
         <v>1</v>
       </c>
       <c r="H28" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K28" s="20">
+        <v>0</v>
+      </c>
+      <c r="K28" s="44">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="L28" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="M28" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="N28" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="O28" s="44">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P28" s="21"/>
-    </row>
-    <row r="29" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L28" s="21"/>
+    </row>
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" s="32"/>
       <c r="B29" s="39" t="s">
         <v>51</v>
@@ -9507,44 +9181,23 @@
         <v>5</v>
       </c>
       <c r="G29" s="20">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H29" s="20">
-        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N29" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O29" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P29" s="21"/>
-    </row>
-    <row r="30" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="K29" s="44">
+        <v>0</v>
+      </c>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="32"/>
       <c r="B30" s="39" t="s">
         <v>84</v>
@@ -9559,48 +9212,29 @@
         <v>18</v>
       </c>
       <c r="F30" s="20">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G30" s="20">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I30" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J30" s="20">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K30" s="20">
+        <v>0</v>
+      </c>
+      <c r="K30" s="44">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L30" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M30" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N30" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O30" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P30" s="21"/>
-    </row>
-    <row r="31" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="L30" s="21"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="32"/>
       <c r="B31" s="40" t="s">
         <v>52</v>
@@ -9627,36 +9261,19 @@
         <v>1</v>
       </c>
       <c r="I31" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K31" s="20">
+        <v>0</v>
+      </c>
+      <c r="K31" s="44">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="L31" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="M31" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="N31" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="O31" s="44">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P31" s="21"/>
-    </row>
-    <row r="32" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L31" s="21"/>
+    </row>
+    <row r="32" spans="1:12" ht="30">
       <c r="A32" s="32"/>
       <c r="B32" s="40" t="s">
         <v>53</v>
@@ -9683,36 +9300,19 @@
         <v>5</v>
       </c>
       <c r="I32" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J32" s="20">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K32" s="20">
+        <v>0</v>
+      </c>
+      <c r="K32" s="44">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L32" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M32" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N32" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O32" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P32" s="21"/>
-    </row>
-    <row r="33" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L32" s="21"/>
+    </row>
+    <row r="33" spans="1:12" ht="30">
       <c r="A33" s="33"/>
       <c r="B33" s="39" t="s">
         <v>54</v>
@@ -9727,48 +9327,31 @@
         <v>18</v>
       </c>
       <c r="F33" s="20">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G33" s="20">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H33" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33" s="20">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="K33" s="20">
+        <v>0</v>
+      </c>
+      <c r="K33" s="44">
         <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L33" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="M33" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="N33" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="O33" s="44">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="P33" s="21"/>
-    </row>
-    <row r="34" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L33" s="21"/>
+    </row>
+    <row r="34" spans="1:12" ht="30">
       <c r="A34" s="33"/>
       <c r="B34" s="40" t="s">
         <v>55</v>
@@ -9791,40 +9374,21 @@
         <v>5</v>
       </c>
       <c r="H34" s="20">
+        <v>7</v>
+      </c>
+      <c r="I34" s="20">
+        <v>3</v>
+      </c>
+      <c r="J34" s="20">
+        <v>0</v>
+      </c>
+      <c r="K34" s="44">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="I34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="J34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N34" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O34" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P34" s="21"/>
-    </row>
-    <row r="35" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="L34" s="21"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="33"/>
       <c r="B35" s="40" t="s">
         <v>93</v>
@@ -9839,48 +9403,29 @@
         <v>18</v>
       </c>
       <c r="F35" s="20">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G35" s="20">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H35" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I35" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J35" s="20">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K35" s="20">
+        <v>0</v>
+      </c>
+      <c r="K35" s="44">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L35" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M35" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N35" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O35" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P35" s="21"/>
-    </row>
-    <row r="36" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="L35" s="21"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="33"/>
       <c r="B36" s="40" t="s">
         <v>87</v>
@@ -9907,36 +9452,18 @@
         <v>3</v>
       </c>
       <c r="I36" s="20">
+        <v>1</v>
+      </c>
+      <c r="J36" s="20">
+        <v>0</v>
+      </c>
+      <c r="K36" s="44">
         <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="J36" s="20">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="K36" s="20">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="L36" s="20">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="M36" s="20">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="N36" s="20">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="O36" s="44">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="P36" s="21"/>
-    </row>
-    <row r="37" spans="1:16" ht="30">
+        <v>0</v>
+      </c>
+      <c r="L36" s="21"/>
+    </row>
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="33"/>
       <c r="B37" s="40" t="s">
         <v>88</v>
@@ -9967,32 +9494,14 @@
         <v>4</v>
       </c>
       <c r="J37" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="K37" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="L37" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="M37" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="N37" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="O37" s="44">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="P37" s="21"/>
-    </row>
-    <row r="38" spans="1:16">
+        <v>2</v>
+      </c>
+      <c r="K37" s="44">
+        <v>0</v>
+      </c>
+      <c r="L37" s="21"/>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="33"/>
       <c r="B38" s="39" t="s">
         <v>89</v>
@@ -10026,29 +9535,12 @@
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="K38" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L38" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="M38" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="N38" s="20">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="O38" s="44">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="P38" s="21"/>
-    </row>
-    <row r="39" spans="1:16" ht="45">
+      <c r="K38" s="44">
+        <v>0</v>
+      </c>
+      <c r="L38" s="21"/>
+    </row>
+    <row r="39" spans="1:12" ht="45">
       <c r="A39" s="33"/>
       <c r="B39" s="39" t="s">
         <v>44</v>
@@ -10079,32 +9571,15 @@
         <v>1</v>
       </c>
       <c r="J39" s="20">
+        <v>0</v>
+      </c>
+      <c r="K39" s="44">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K39" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="L39" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="M39" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="N39" s="20">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="O39" s="44">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P39" s="21"/>
-    </row>
-    <row r="40" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="L39" s="21"/>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="33"/>
       <c r="B40" s="39" t="s">
         <v>95</v>
@@ -10135,32 +9610,14 @@
         <v>5</v>
       </c>
       <c r="J40" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="K40" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="L40" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="M40" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="N40" s="20">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="O40" s="44">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="P40" s="21"/>
-    </row>
-    <row r="41" spans="1:16" ht="16" thickBot="1">
+        <v>3</v>
+      </c>
+      <c r="K40" s="44">
+        <v>0</v>
+      </c>
+      <c r="L40" s="21"/>
+    </row>
+    <row r="41" spans="1:12" ht="16" thickBot="1">
       <c r="A41" s="33"/>
       <c r="B41" s="109" t="s">
         <v>94</v>
@@ -10194,29 +9651,12 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="K41" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="L41" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="M41" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="N41" s="20">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="O41" s="44">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="P41" s="21"/>
-    </row>
-    <row r="42" spans="1:16" ht="16" thickBot="1">
+      <c r="K41" s="44">
+        <v>0</v>
+      </c>
+      <c r="L41" s="21"/>
+    </row>
+    <row r="42" spans="1:12" ht="16" thickBot="1">
       <c r="A42" s="12" t="s">
         <v>15</v>
       </c>
@@ -10228,53 +9668,37 @@
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17">
-        <f t="shared" ref="F42:O42" si="9">SUM(F26:F41)</f>
-        <v>52</v>
+        <f t="shared" ref="F42:K42" si="9">SUM(F26:F41)</f>
+        <v>47</v>
       </c>
       <c r="G42" s="17">
         <f t="shared" si="9"/>
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H42" s="17">
         <f t="shared" si="9"/>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I42" s="17">
         <f t="shared" si="9"/>
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J42" s="17">
         <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-      <c r="K42" s="17">
+        <v>12</v>
+      </c>
+      <c r="K42" s="18">
         <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-      <c r="L42" s="17">
-        <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-      <c r="M42" s="17">
-        <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-      <c r="N42" s="17">
-        <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-      <c r="O42" s="18">
-        <f t="shared" si="9"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="18">
       <c r="D45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="62"/>
     </row>
-    <row r="46" spans="1:16" ht="18">
+    <row r="46" spans="1:12" ht="18">
       <c r="D46" s="95" t="s">
         <v>22</v>
       </c>
@@ -10282,7 +9706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="18">
+    <row r="47" spans="1:12" ht="18">
       <c r="D47" s="95" t="s">
         <v>24</v>
       </c>
@@ -10290,7 +9714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="18">
+    <row r="48" spans="1:12" ht="18">
       <c r="D48" s="95" t="s">
         <v>23</v>
       </c>

</xml_diff>